<commit_message>
Latest DFMEA of AMT project.
</commit_message>
<xml_diff>
--- a/AMT HALL EFFECT/05_Documents/FMEA/BOUNDARY_DIAGRAM_AMT.xlsx
+++ b/AMT HALL EFFECT/05_Documents/FMEA/BOUNDARY_DIAGRAM_AMT.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Embdes_GitLab\LUMAX\amt\AMT HALL EFFECT\05_Documents\FMEA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\New Volume\Embdes_Final\LUMAX\AMT_Hall_Effect\AMT_20 pin microcontroller\Documents\FMEA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6255" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6255"/>
   </bookViews>
   <sheets>
     <sheet name="BD_AMT" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="284">
   <si>
     <t>BOUNDARY DIAGRAM - TATA AMT NEXON</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>Ekta Bhayana</t>
-  </si>
-  <si>
-    <t>25.09.19</t>
   </si>
   <si>
     <t>Date</t>
@@ -1073,7 +1070,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1115,6 +1112,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1130,8 +1130,13 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1158,13 +1163,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>168087</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>22412</xdr:rowOff>
+      <xdr:rowOff>22411</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>358589</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>145676</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1173,8 +1178,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="168087" y="784412"/>
-          <a:ext cx="10163737" cy="3597088"/>
+          <a:off x="168087" y="784411"/>
+          <a:ext cx="10163737" cy="4123765"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2267,7 +2272,7 @@
                 </a:schemeClr>
               </a:solidFill>
             </a:rPr>
-            <a:t>ECU</a:t>
+            <a:t>TCU</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2751,6 +2756,129 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>123266</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>123264</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>146239</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>66114</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="Rounded Rectangle 26"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4650442" y="4504764"/>
+          <a:ext cx="1838326" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1200" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Mechanical Fixture</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-IN" sz="1200" b="1">
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>402750</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>14654</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>402981</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>132536</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="Straight Arrow Connector 27"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5553577" y="4205654"/>
+          <a:ext cx="231" cy="308382"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="002060"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2761,13 +2889,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>168087</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>171449</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>358589</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2776,8 +2904,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="168087" y="742950"/>
-          <a:ext cx="12096752" cy="3638550"/>
+          <a:off x="168087" y="742949"/>
+          <a:ext cx="12096752" cy="4200525"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3870,7 +3998,7 @@
                 </a:schemeClr>
               </a:solidFill>
             </a:rPr>
-            <a:t>ECU</a:t>
+            <a:t>TCU</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -3881,13 +4009,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>660224</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>114832</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3931,13 +4059,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>60614</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>104776</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>676275</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>108239</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -4087,13 +4215,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>120361</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>134216</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>678006</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>137682</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -4137,13 +4265,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>637190</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>105103</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -4189,13 +4317,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>250362</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4622,7 +4750,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-IN" sz="1100"/>
-            <a:t>\T(-2)\E(-1)</a:t>
+            <a:t>\T(0)\E(-1)</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -4679,7 +4807,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-IN" sz="1100"/>
-            <a:t>Vo(+2)\I(+2)\T(-2)\E(-1)</a:t>
+            <a:t>Vo(+2)\I(+2)\T(0)\E(-1)</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -4736,7 +4864,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-IN" sz="1100"/>
-            <a:t>Vo(+2)\I(+2)\T(-2)\E(-1)</a:t>
+            <a:t>Vo(+2)\I(+2)\T(0)\E(-1)</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -4793,7 +4921,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-IN" sz="1100"/>
-            <a:t>Vo(+2)\I(+2)\T(-2)\E(-1)\Ss(+2)</a:t>
+            <a:t>Vo(+2),I(+2),T(0),E(-1),Ss(+2)</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -4850,7 +4978,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-IN" sz="1100"/>
-            <a:t>Vo(+2)\I(+2)\T(-2)\E(-1)\Sg(+2)</a:t>
+            <a:t>Vo(+2),I(+2),T(0),E(-1),Sg(+2)</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -4907,14 +5035,14 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-IN" sz="1100"/>
-            <a:t>Vo(+2)\I(+2)\T(-2)</a:t>
+            <a:t>Vo(+2),I(+2),T(0)</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-IN" sz="1100"/>
-            <a:t>\E(-1)\Sg(+2)</a:t>
+            <a:t>,E(-1),Sg(+2)</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -4978,7 +5106,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-IN" sz="1100"/>
-            <a:t>\T(-2)\E(-1)</a:t>
+            <a:t>\T(0)\E(-1)</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -5035,14 +5163,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-IN" sz="1100"/>
-            <a:t>T(-2)</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-IN" sz="1100"/>
-            <a:t>\E(-1)\Sg(+2)</a:t>
+            <a:t>E(-1),Sg(+2)</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -5152,7 +5273,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-IN" sz="1100"/>
-            <a:t>Mf(+2)\T(-2)\</a:t>
+            <a:t>Mf(+2)\T(0)\</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -5170,13 +5291,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>628090</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>106456</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -5195,6 +5316,129 @@
         <a:ln>
           <a:solidFill>
             <a:srgbClr val="00B050"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>649942</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>78441</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>64435</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>21291</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="52" name="Rounded Rectangle 51"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5871883" y="4459941"/>
+          <a:ext cx="1834964" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1200" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Mechanical Fixture</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-IN" sz="1200" b="1">
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>750832</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>13139</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>768569</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>85397</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="54" name="Straight Arrow Connector 53"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="6735160" y="4204139"/>
+          <a:ext cx="17737" cy="262758"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="002060"/>
           </a:solidFill>
           <a:tailEnd type="triangle"/>
         </a:ln>
@@ -5482,10 +5726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T23"/>
+  <dimension ref="A1:T30"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T17" sqref="T17"/>
+    <sheetView tabSelected="1" topLeftCell="C10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5510,7 +5754,7 @@
       <c r="S1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="T1" s="24" t="s">
         <v>8</v>
       </c>
     </row>
@@ -5524,10 +5768,10 @@
       <c r="M2" s="13"/>
       <c r="N2" s="13"/>
       <c r="S2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="T2" s="7" t="s">
         <v>9</v>
+      </c>
+      <c r="T2" s="23">
+        <v>43747</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -5787,7 +6031,7 @@
       <c r="R17" s="16"/>
       <c r="S17" s="1"/>
       <c r="T17" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="18" spans="1:20">
@@ -5910,12 +6154,160 @@
       <c r="Q23" s="16"/>
       <c r="R23" s="16"/>
     </row>
+    <row r="24" spans="1:20">
+      <c r="A24" s="16"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="16"/>
+      <c r="N24" s="16"/>
+      <c r="O24" s="16"/>
+      <c r="P24" s="16"/>
+      <c r="Q24" s="16"/>
+      <c r="R24" s="16"/>
+      <c r="S24" s="16"/>
+    </row>
+    <row r="25" spans="1:20">
+      <c r="A25" s="16"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="16"/>
+      <c r="N25" s="16"/>
+      <c r="O25" s="16"/>
+      <c r="P25" s="16"/>
+      <c r="Q25" s="16"/>
+      <c r="R25" s="16"/>
+      <c r="S25" s="16"/>
+    </row>
+    <row r="26" spans="1:20">
+      <c r="A26" s="16"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="16"/>
+      <c r="N26" s="16"/>
+      <c r="O26" s="16"/>
+      <c r="P26" s="16"/>
+      <c r="Q26" s="16"/>
+      <c r="R26" s="16"/>
+      <c r="S26" s="16"/>
+    </row>
+    <row r="27" spans="1:20">
+      <c r="A27" s="16"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="16"/>
+      <c r="O27" s="16"/>
+      <c r="P27" s="16"/>
+      <c r="Q27" s="16"/>
+      <c r="R27" s="16"/>
+      <c r="S27" s="16"/>
+    </row>
+    <row r="28" spans="1:20">
+      <c r="A28" s="16"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="16"/>
+      <c r="N28" s="16"/>
+      <c r="O28" s="16"/>
+      <c r="P28" s="16"/>
+      <c r="Q28" s="16"/>
+      <c r="R28" s="16"/>
+      <c r="S28" s="16"/>
+    </row>
+    <row r="29" spans="1:20">
+      <c r="A29" s="16"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="16"/>
+      <c r="M29" s="16"/>
+      <c r="N29" s="16"/>
+      <c r="O29" s="16"/>
+      <c r="P29" s="16"/>
+      <c r="Q29" s="16"/>
+      <c r="R29" s="16"/>
+      <c r="S29" s="16"/>
+    </row>
+    <row r="30" spans="1:20">
+      <c r="A30" s="16"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="16"/>
+      <c r="K30" s="16"/>
+      <c r="L30" s="16"/>
+      <c r="M30" s="16"/>
+      <c r="N30" s="16"/>
+      <c r="O30" s="16"/>
+      <c r="P30" s="16"/>
+      <c r="Q30" s="16"/>
+      <c r="R30" s="16"/>
+      <c r="S30" s="16"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="G1:N3"/>
     <mergeCell ref="T14:T15"/>
     <mergeCell ref="S14:S15"/>
     <mergeCell ref="A7:R23"/>
+    <mergeCell ref="A24:S30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5925,10 +6317,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T107"/>
+  <dimension ref="A1:T110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5941,6 +6333,7 @@
     <col min="8" max="8" width="11.42578125" customWidth="1"/>
     <col min="9" max="9" width="15.7109375" customWidth="1"/>
     <col min="10" max="10" width="9.140625" customWidth="1"/>
+    <col min="20" max="20" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="9.140625" customWidth="1"/>
     <col min="23" max="23" width="29.85546875" customWidth="1"/>
     <col min="24" max="24" width="25" customWidth="1"/>
@@ -5978,10 +6371,10 @@
       <c r="M2" s="13"/>
       <c r="N2" s="13"/>
       <c r="S2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="T2" s="7" t="s">
         <v>9</v>
+      </c>
+      <c r="T2" s="7">
+        <v>43747</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -6334,750 +6727,764 @@
       <c r="Q23" s="16"/>
       <c r="R23" s="16"/>
     </row>
+    <row r="24" spans="1:18">
+      <c r="A24" s="16"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="16"/>
+      <c r="N24" s="16"/>
+      <c r="O24" s="16"/>
+      <c r="P24" s="16"/>
+      <c r="Q24" s="16"/>
+      <c r="R24" s="16"/>
+    </row>
     <row r="25" spans="1:18">
-      <c r="H25" s="2" t="s">
+      <c r="A25" s="16"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="16"/>
+      <c r="N25" s="16"/>
+      <c r="O25" s="16"/>
+      <c r="P25" s="16"/>
+      <c r="Q25" s="16"/>
+      <c r="R25" s="16"/>
+    </row>
+    <row r="26" spans="1:18">
+      <c r="A26" s="16"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="16"/>
+      <c r="N26" s="16"/>
+      <c r="O26" s="16"/>
+      <c r="P26" s="16"/>
+      <c r="Q26" s="16"/>
+      <c r="R26" s="16"/>
+    </row>
+    <row r="28" spans="1:18">
+      <c r="H28" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I25" s="2" t="s">
+      <c r="I28" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:18">
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-    </row>
-    <row r="27" spans="1:18">
-      <c r="H27" s="1"/>
-      <c r="I27" s="3" t="s">
+    <row r="29" spans="1:18">
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="1:18">
+      <c r="H30" s="1"/>
+      <c r="I30" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="L27" s="20" t="s">
-        <v>284</v>
-      </c>
-      <c r="M27" s="20"/>
-      <c r="N27" s="20"/>
-      <c r="O27" s="20"/>
-      <c r="P27" s="20"/>
-      <c r="Q27" s="20"/>
-    </row>
-    <row r="28" spans="1:18">
-      <c r="H28" s="1"/>
-      <c r="I28" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="L28" s="20"/>
-      <c r="M28" s="20"/>
-      <c r="N28" s="20"/>
-      <c r="O28" s="20"/>
-      <c r="P28" s="20"/>
-      <c r="Q28" s="20"/>
-    </row>
-    <row r="29" spans="1:18">
-      <c r="H29" s="15"/>
-      <c r="I29" s="22" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" ht="32.25" customHeight="1">
-      <c r="H30" s="15"/>
-      <c r="I30" s="22"/>
+      <c r="L30" s="21" t="s">
+        <v>283</v>
+      </c>
+      <c r="M30" s="21"/>
+      <c r="N30" s="21"/>
+      <c r="O30" s="21"/>
+      <c r="P30" s="21"/>
+      <c r="Q30" s="21"/>
     </row>
     <row r="31" spans="1:18">
       <c r="H31" s="1"/>
-      <c r="I31" s="4" t="s">
+      <c r="I31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="L31" s="21"/>
+      <c r="M31" s="21"/>
+      <c r="N31" s="21"/>
+      <c r="O31" s="21"/>
+      <c r="P31" s="21"/>
+      <c r="Q31" s="21"/>
+    </row>
+    <row r="32" spans="1:18">
+      <c r="H32" s="15"/>
+      <c r="I32" s="17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" ht="32.25" customHeight="1">
+      <c r="H33" s="15"/>
+      <c r="I33" s="17"/>
+    </row>
+    <row r="34" spans="2:9">
+      <c r="H34" s="1"/>
+      <c r="I34" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:18">
-      <c r="H32" s="1"/>
-      <c r="I32" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="34" spans="2:9" ht="15.75" thickBot="1"/>
-    <row r="35" spans="2:9" ht="16.5" thickBot="1">
-      <c r="B35" s="17" t="s">
+    <row r="35" spans="2:9">
+      <c r="H35" s="1"/>
+      <c r="I35" s="4" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" ht="15.75" thickBot="1"/>
+    <row r="38" spans="2:9" ht="16.5" thickBot="1">
+      <c r="B38" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="19"/>
+    </row>
+    <row r="39" spans="2:9" ht="16.5" thickBot="1">
+      <c r="B39" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="21"/>
-      <c r="I35" s="18"/>
-    </row>
-    <row r="36" spans="2:9" ht="16.5" thickBot="1">
-      <c r="B36" s="17" t="s">
+      <c r="C39" s="19"/>
+      <c r="D39" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="19" t="s">
+      <c r="E39" s="19"/>
+      <c r="F39" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="E36" s="18"/>
-      <c r="F36" s="19" t="s">
+      <c r="G39" s="19"/>
+      <c r="H39" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="G36" s="18"/>
-      <c r="H36" s="19" t="s">
+      <c r="I39" s="19"/>
+    </row>
+    <row r="40" spans="2:9" ht="32.25" thickBot="1">
+      <c r="B40" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="I36" s="18"/>
-    </row>
-    <row r="37" spans="2:9" ht="32.25" thickBot="1">
-      <c r="B37" s="8" t="s">
+      <c r="C40" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="D40" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D37" s="9" t="s">
+      <c r="E40" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E37" s="9" t="s">
+      <c r="F40" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F37" s="9" t="s">
+      <c r="G40" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="G37" s="9" t="s">
+      <c r="H40" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H37" s="9" t="s">
+      <c r="I40" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="I37" s="9" t="s">
+    </row>
+    <row r="41" spans="2:9" ht="16.5" thickBot="1">
+      <c r="B41" s="8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="38" spans="2:9" ht="16.5" thickBot="1">
-      <c r="B38" s="8" t="s">
+      <c r="C41" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="D41" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D38" s="9" t="s">
+      <c r="E41" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E38" s="9" t="s">
+      <c r="F41" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F38" s="9" t="s">
+      <c r="G41" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G38" s="9" t="s">
+      <c r="H41" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H38" s="9" t="s">
+      <c r="I41" s="9" t="s">
         <v>30</v>
-      </c>
-      <c r="I38" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="39" spans="2:9" ht="16.5" thickBot="1">
-      <c r="B39" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E39" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F39" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="G39" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="H39" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="I39" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="40" spans="2:9" ht="16.5" thickBot="1">
-      <c r="B40" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F40" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="G40" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="H40" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="I40" s="9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="41" spans="2:9" ht="32.25" thickBot="1">
-      <c r="B41" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="F41" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G41" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="H41" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="I41" s="9" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="42" spans="2:9" ht="16.5" thickBot="1">
       <c r="B42" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H42" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I42" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" ht="16.5" thickBot="1">
+      <c r="B43" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H43" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I43" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" ht="32.25" thickBot="1">
+      <c r="B44" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G44" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="H44" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="I44" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" ht="16.5" thickBot="1">
+      <c r="B45" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C42" s="9" t="s">
+      <c r="D45" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D42" s="9" t="s">
+      <c r="E45" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E42" s="9" t="s">
+      <c r="F45" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="F42" s="9" t="s">
+      <c r="G45" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H45" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="G42" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H42" s="9" t="s">
+      <c r="I45" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="I42" s="9" t="s">
+    </row>
+    <row r="46" spans="2:9" ht="32.25" thickBot="1">
+      <c r="B46" s="8" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="43" spans="2:9" ht="32.25" thickBot="1">
-      <c r="B43" s="8" t="s">
+      <c r="C46" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C43" s="9" t="s">
+      <c r="D46" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D43" s="9" t="s">
+      <c r="E46" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E43" s="9" t="s">
+      <c r="F46" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="F43" s="9" t="s">
+      <c r="G46" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G43" s="9" t="s">
+      <c r="H46" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="H43" s="9" t="s">
+      <c r="I46" s="9" t="s">
         <v>69</v>
-      </c>
-      <c r="I43" s="9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="44" spans="2:9" ht="16.5" thickBot="1">
-      <c r="B44" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D44" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F44" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="G44" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="H44" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="I44" s="9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="45" spans="2:9" ht="48" thickBot="1">
-      <c r="B45" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="D45" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="E45" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="F45" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="G45" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="H45" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="I45" s="9" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="46" spans="2:9" ht="16.5" thickBot="1">
-      <c r="B46" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="E46" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="F46" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="G46" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="H46" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="I46" s="9" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="47" spans="2:9" ht="16.5" thickBot="1">
       <c r="B47" s="8" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>96</v>
+        <v>71</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>98</v>
+        <v>73</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>99</v>
+        <v>74</v>
       </c>
       <c r="G47" s="9" t="s">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="H47" s="9" t="s">
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="I47" s="9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="48" spans="2:9" ht="32.25" thickBot="1">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" ht="48" thickBot="1">
       <c r="B48" s="8" t="s">
-        <v>103</v>
+        <v>78</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>104</v>
+        <v>79</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>105</v>
+        <v>80</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>106</v>
+        <v>81</v>
       </c>
       <c r="F48" s="9" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="G48" s="9" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="H48" s="9" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="I48" s="9" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="49" spans="2:9" ht="16.5" thickBot="1">
       <c r="B49" s="8" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="G49" s="9" t="s">
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="H49" s="9" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="I49" s="9" t="s">
-        <v>118</v>
+        <v>93</v>
       </c>
     </row>
     <row r="50" spans="2:9" ht="16.5" thickBot="1">
       <c r="B50" s="8" t="s">
-        <v>119</v>
+        <v>94</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>121</v>
+        <v>96</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
+        <v>97</v>
+      </c>
+      <c r="F50" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="G50" s="9" t="s">
+        <v>99</v>
+      </c>
       <c r="H50" s="9" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="I50" s="9" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="51" spans="2:9" ht="16.5" thickBot="1">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" ht="32.25" thickBot="1">
       <c r="B51" s="8" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="F51" s="9"/>
-      <c r="G51" s="9"/>
+        <v>105</v>
+      </c>
+      <c r="F51" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="G51" s="9" t="s">
+        <v>107</v>
+      </c>
       <c r="H51" s="9" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="I51" s="9" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
     </row>
     <row r="52" spans="2:9" ht="16.5" thickBot="1">
       <c r="B52" s="8" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="F52" s="9"/>
-      <c r="G52" s="9"/>
+        <v>113</v>
+      </c>
+      <c r="F52" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="G52" s="9" t="s">
+        <v>115</v>
+      </c>
       <c r="H52" s="9" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="I52" s="9" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
     </row>
     <row r="53" spans="2:9" ht="16.5" thickBot="1">
       <c r="B53" s="8" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="F53" s="9"/>
       <c r="G53" s="9"/>
       <c r="H53" s="9" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="I53" s="9" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="54" spans="2:9" ht="32.25" thickBot="1">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" ht="16.5" thickBot="1">
       <c r="B54" s="8" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
       <c r="F54" s="9"/>
       <c r="G54" s="9"/>
       <c r="H54" s="9" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="I54" s="9" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="55" spans="2:9" ht="32.25" thickBot="1">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" ht="16.5" thickBot="1">
       <c r="B55" s="8" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="F55" s="9"/>
       <c r="G55" s="9"/>
       <c r="H55" s="9" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="I55" s="9" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
     </row>
     <row r="56" spans="2:9" ht="16.5" thickBot="1">
       <c r="B56" s="8" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="F56" s="9"/>
       <c r="G56" s="9"/>
       <c r="H56" s="9" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="I56" s="9" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
     </row>
     <row r="57" spans="2:9" ht="32.25" thickBot="1">
       <c r="B57" s="8" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
       <c r="F57" s="9"/>
       <c r="G57" s="9"/>
       <c r="H57" s="9" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="I57" s="9" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
     </row>
     <row r="58" spans="2:9" ht="32.25" thickBot="1">
       <c r="B58" s="8" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>168</v>
+        <v>149</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="F58" s="9"/>
       <c r="G58" s="9"/>
       <c r="H58" s="9" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="I58" s="9" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="59" spans="2:9" ht="32.25" thickBot="1">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="59" spans="2:9" ht="16.5" thickBot="1">
       <c r="B59" s="8" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="F59" s="9"/>
       <c r="G59" s="9"/>
       <c r="H59" s="9" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="I59" s="9" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="60" spans="2:9" ht="16.5" thickBot="1">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="60" spans="2:9" ht="32.25" thickBot="1">
       <c r="B60" s="8" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="F60" s="9"/>
       <c r="G60" s="9"/>
-      <c r="H60" s="9"/>
-      <c r="I60" s="9"/>
+      <c r="H60" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="I60" s="9" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="61" spans="2:9" ht="32.25" thickBot="1">
       <c r="B61" s="8" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
       <c r="F61" s="9"/>
       <c r="G61" s="9"/>
-      <c r="H61" s="9"/>
-      <c r="I61" s="9"/>
+      <c r="H61" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="I61" s="9" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="62" spans="2:9" ht="32.25" thickBot="1">
       <c r="B62" s="8" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="D62" s="9" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="F62" s="9"/>
       <c r="G62" s="9"/>
-      <c r="H62" s="9"/>
-      <c r="I62" s="9"/>
+      <c r="H62" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="I62" s="9" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="63" spans="2:9" ht="16.5" thickBot="1">
       <c r="B63" s="8" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="F63" s="9"/>
       <c r="G63" s="9"/>
       <c r="H63" s="9"/>
       <c r="I63" s="9"/>
     </row>
-    <row r="64" spans="2:9" ht="16.5" thickBot="1">
+    <row r="64" spans="2:9" ht="32.25" thickBot="1">
       <c r="B64" s="8" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="D64" s="10"/>
-      <c r="E64" s="9"/>
+        <v>183</v>
+      </c>
+      <c r="D64" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="E64" s="9" t="s">
+        <v>185</v>
+      </c>
       <c r="F64" s="9"/>
       <c r="G64" s="9"/>
       <c r="H64" s="9"/>
       <c r="I64" s="9"/>
     </row>
-    <row r="65" spans="2:9" ht="16.5" thickBot="1">
+    <row r="65" spans="2:9" ht="32.25" thickBot="1">
       <c r="B65" s="8" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="D65" s="9"/>
-      <c r="E65" s="9"/>
+        <v>187</v>
+      </c>
+      <c r="D65" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>189</v>
+      </c>
       <c r="F65" s="9"/>
       <c r="G65" s="9"/>
       <c r="H65" s="9"/>
@@ -7085,13 +7492,17 @@
     </row>
     <row r="66" spans="2:9" ht="16.5" thickBot="1">
       <c r="B66" s="8" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>200</v>
-      </c>
-      <c r="D66" s="9"/>
-      <c r="E66" s="9"/>
+        <v>191</v>
+      </c>
+      <c r="D66" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="E66" s="9" t="s">
+        <v>193</v>
+      </c>
       <c r="F66" s="9"/>
       <c r="G66" s="9"/>
       <c r="H66" s="9"/>
@@ -7099,24 +7510,24 @@
     </row>
     <row r="67" spans="2:9" ht="16.5" thickBot="1">
       <c r="B67" s="8" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="D67" s="9"/>
+        <v>195</v>
+      </c>
+      <c r="D67" s="10"/>
       <c r="E67" s="9"/>
       <c r="F67" s="9"/>
       <c r="G67" s="9"/>
       <c r="H67" s="9"/>
       <c r="I67" s="9"/>
     </row>
-    <row r="68" spans="2:9" ht="48" thickBot="1">
+    <row r="68" spans="2:9" ht="16.5" thickBot="1">
       <c r="B68" s="8" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="D68" s="9"/>
       <c r="E68" s="9"/>
@@ -7127,10 +7538,10 @@
     </row>
     <row r="69" spans="2:9" ht="16.5" thickBot="1">
       <c r="B69" s="8" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="D69" s="9"/>
       <c r="E69" s="9"/>
@@ -7139,12 +7550,12 @@
       <c r="H69" s="9"/>
       <c r="I69" s="9"/>
     </row>
-    <row r="70" spans="2:9" ht="32.25" thickBot="1">
+    <row r="70" spans="2:9" ht="16.5" thickBot="1">
       <c r="B70" s="8" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="D70" s="9"/>
       <c r="E70" s="9"/>
@@ -7153,12 +7564,12 @@
       <c r="H70" s="9"/>
       <c r="I70" s="9"/>
     </row>
-    <row r="71" spans="2:9" ht="32.25" thickBot="1">
+    <row r="71" spans="2:9" ht="48" thickBot="1">
       <c r="B71" s="8" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="D71" s="9"/>
       <c r="E71" s="9"/>
@@ -7169,10 +7580,10 @@
     </row>
     <row r="72" spans="2:9" ht="16.5" thickBot="1">
       <c r="B72" s="8" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="D72" s="9"/>
       <c r="E72" s="9"/>
@@ -7183,10 +7594,10 @@
     </row>
     <row r="73" spans="2:9" ht="32.25" thickBot="1">
       <c r="B73" s="8" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="D73" s="9"/>
       <c r="E73" s="9"/>
@@ -7195,12 +7606,12 @@
       <c r="H73" s="9"/>
       <c r="I73" s="9"/>
     </row>
-    <row r="74" spans="2:9" ht="16.5" thickBot="1">
+    <row r="74" spans="2:9" ht="32.25" thickBot="1">
       <c r="B74" s="8" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="D74" s="9"/>
       <c r="E74" s="9"/>
@@ -7211,10 +7622,10 @@
     </row>
     <row r="75" spans="2:9" ht="16.5" thickBot="1">
       <c r="B75" s="8" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="D75" s="9"/>
       <c r="E75" s="9"/>
@@ -7223,12 +7634,12 @@
       <c r="H75" s="9"/>
       <c r="I75" s="9"/>
     </row>
-    <row r="76" spans="2:9" ht="16.5" thickBot="1">
+    <row r="76" spans="2:9" ht="32.25" thickBot="1">
       <c r="B76" s="8" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="D76" s="9"/>
       <c r="E76" s="9"/>
@@ -7237,12 +7648,12 @@
       <c r="H76" s="9"/>
       <c r="I76" s="9"/>
     </row>
-    <row r="77" spans="2:9" ht="32.25" thickBot="1">
+    <row r="77" spans="2:9" ht="16.5" thickBot="1">
       <c r="B77" s="8" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="D77" s="9"/>
       <c r="E77" s="9"/>
@@ -7253,10 +7664,10 @@
     </row>
     <row r="78" spans="2:9" ht="16.5" thickBot="1">
       <c r="B78" s="8" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="D78" s="9"/>
       <c r="E78" s="9"/>
@@ -7265,12 +7676,12 @@
       <c r="H78" s="9"/>
       <c r="I78" s="9"/>
     </row>
-    <row r="79" spans="2:9" ht="32.25" thickBot="1">
+    <row r="79" spans="2:9" ht="16.5" thickBot="1">
       <c r="B79" s="8" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="D79" s="9"/>
       <c r="E79" s="9"/>
@@ -7279,12 +7690,12 @@
       <c r="H79" s="9"/>
       <c r="I79" s="9"/>
     </row>
-    <row r="80" spans="2:9" ht="16.5" thickBot="1">
+    <row r="80" spans="2:9" ht="32.25" thickBot="1">
       <c r="B80" s="8" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="D80" s="9"/>
       <c r="E80" s="9"/>
@@ -7295,10 +7706,10 @@
     </row>
     <row r="81" spans="2:9" ht="16.5" thickBot="1">
       <c r="B81" s="8" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="D81" s="9"/>
       <c r="E81" s="9"/>
@@ -7307,12 +7718,12 @@
       <c r="H81" s="9"/>
       <c r="I81" s="9"/>
     </row>
-    <row r="82" spans="2:9" ht="16.5" thickBot="1">
+    <row r="82" spans="2:9" ht="32.25" thickBot="1">
       <c r="B82" s="8" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="D82" s="9"/>
       <c r="E82" s="9"/>
@@ -7323,10 +7734,10 @@
     </row>
     <row r="83" spans="2:9" ht="16.5" thickBot="1">
       <c r="B83" s="8" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="D83" s="9"/>
       <c r="E83" s="9"/>
@@ -7337,10 +7748,10 @@
     </row>
     <row r="84" spans="2:9" ht="16.5" thickBot="1">
       <c r="B84" s="8" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="D84" s="9"/>
       <c r="E84" s="9"/>
@@ -7349,12 +7760,12 @@
       <c r="H84" s="9"/>
       <c r="I84" s="9"/>
     </row>
-    <row r="85" spans="2:9" ht="32.25" thickBot="1">
+    <row r="85" spans="2:9" ht="16.5" thickBot="1">
       <c r="B85" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="D85" s="9"/>
       <c r="E85" s="9"/>
@@ -7363,12 +7774,12 @@
       <c r="H85" s="9"/>
       <c r="I85" s="9"/>
     </row>
-    <row r="86" spans="2:9" ht="32.25" thickBot="1">
+    <row r="86" spans="2:9" ht="16.5" thickBot="1">
       <c r="B86" s="8" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="D86" s="9"/>
       <c r="E86" s="9"/>
@@ -7379,10 +7790,10 @@
     </row>
     <row r="87" spans="2:9" ht="16.5" thickBot="1">
       <c r="B87" s="8" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="C87" s="9" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="D87" s="9"/>
       <c r="E87" s="9"/>
@@ -7393,10 +7804,10 @@
     </row>
     <row r="88" spans="2:9" ht="32.25" thickBot="1">
       <c r="B88" s="8" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="C88" s="9" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="D88" s="9"/>
       <c r="E88" s="9"/>
@@ -7407,10 +7818,10 @@
     </row>
     <row r="89" spans="2:9" ht="32.25" thickBot="1">
       <c r="B89" s="8" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="C89" s="9" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="D89" s="9"/>
       <c r="E89" s="9"/>
@@ -7421,10 +7832,10 @@
     </row>
     <row r="90" spans="2:9" ht="16.5" thickBot="1">
       <c r="B90" s="8" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="C90" s="9" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="D90" s="9"/>
       <c r="E90" s="9"/>
@@ -7435,10 +7846,10 @@
     </row>
     <row r="91" spans="2:9" ht="32.25" thickBot="1">
       <c r="B91" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="C91" s="9" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="D91" s="9"/>
       <c r="E91" s="9"/>
@@ -7447,12 +7858,12 @@
       <c r="H91" s="9"/>
       <c r="I91" s="9"/>
     </row>
-    <row r="92" spans="2:9" ht="16.5" thickBot="1">
+    <row r="92" spans="2:9" ht="32.25" thickBot="1">
       <c r="B92" s="8" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="C92" s="9" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="D92" s="9"/>
       <c r="E92" s="9"/>
@@ -7461,12 +7872,12 @@
       <c r="H92" s="9"/>
       <c r="I92" s="9"/>
     </row>
-    <row r="93" spans="2:9" ht="32.25" thickBot="1">
+    <row r="93" spans="2:9" ht="16.5" thickBot="1">
       <c r="B93" s="8" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="C93" s="9" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="D93" s="9"/>
       <c r="E93" s="9"/>
@@ -7477,10 +7888,10 @@
     </row>
     <row r="94" spans="2:9" ht="32.25" thickBot="1">
       <c r="B94" s="8" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="C94" s="9" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="D94" s="9"/>
       <c r="E94" s="9"/>
@@ -7491,10 +7902,10 @@
     </row>
     <row r="95" spans="2:9" ht="16.5" thickBot="1">
       <c r="B95" s="8" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="D95" s="9"/>
       <c r="E95" s="9"/>
@@ -7503,12 +7914,12 @@
       <c r="H95" s="9"/>
       <c r="I95" s="9"/>
     </row>
-    <row r="96" spans="2:9" ht="16.5" thickBot="1">
+    <row r="96" spans="2:9" ht="32.25" thickBot="1">
       <c r="B96" s="8" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="D96" s="9"/>
       <c r="E96" s="9"/>
@@ -7519,10 +7930,10 @@
     </row>
     <row r="97" spans="2:9" ht="32.25" thickBot="1">
       <c r="B97" s="8" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="C97" s="9" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="D97" s="9"/>
       <c r="E97" s="9"/>
@@ -7531,12 +7942,12 @@
       <c r="H97" s="9"/>
       <c r="I97" s="9"/>
     </row>
-    <row r="98" spans="2:9" ht="32.25" thickBot="1">
+    <row r="98" spans="2:9" ht="16.5" thickBot="1">
       <c r="B98" s="8" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="C98" s="9" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="D98" s="9"/>
       <c r="E98" s="9"/>
@@ -7545,12 +7956,12 @@
       <c r="H98" s="9"/>
       <c r="I98" s="9"/>
     </row>
-    <row r="99" spans="2:9" ht="32.25" thickBot="1">
+    <row r="99" spans="2:9" ht="16.5" thickBot="1">
       <c r="B99" s="8" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="C99" s="9" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="D99" s="9"/>
       <c r="E99" s="9"/>
@@ -7561,10 +7972,10 @@
     </row>
     <row r="100" spans="2:9" ht="32.25" thickBot="1">
       <c r="B100" s="8" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="C100" s="9" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="D100" s="9"/>
       <c r="E100" s="9"/>
@@ -7575,10 +7986,10 @@
     </row>
     <row r="101" spans="2:9" ht="32.25" thickBot="1">
       <c r="B101" s="8" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="C101" s="9" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="D101" s="9"/>
       <c r="E101" s="9"/>
@@ -7587,12 +7998,12 @@
       <c r="H101" s="9"/>
       <c r="I101" s="9"/>
     </row>
-    <row r="102" spans="2:9" ht="16.5" thickBot="1">
+    <row r="102" spans="2:9" ht="32.25" thickBot="1">
       <c r="B102" s="8" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="C102" s="9" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="D102" s="9"/>
       <c r="E102" s="9"/>
@@ -7603,10 +8014,10 @@
     </row>
     <row r="103" spans="2:9" ht="32.25" thickBot="1">
       <c r="B103" s="8" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="C103" s="9" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="D103" s="9"/>
       <c r="E103" s="9"/>
@@ -7617,10 +8028,10 @@
     </row>
     <row r="104" spans="2:9" ht="32.25" thickBot="1">
       <c r="B104" s="8" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="C104" s="9" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="D104" s="9"/>
       <c r="E104" s="9"/>
@@ -7629,12 +8040,12 @@
       <c r="H104" s="9"/>
       <c r="I104" s="9"/>
     </row>
-    <row r="105" spans="2:9" ht="32.25" thickBot="1">
+    <row r="105" spans="2:9" ht="16.5" thickBot="1">
       <c r="B105" s="8" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="C105" s="9" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="D105" s="9"/>
       <c r="E105" s="9"/>
@@ -7645,10 +8056,10 @@
     </row>
     <row r="106" spans="2:9" ht="32.25" thickBot="1">
       <c r="B106" s="8" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="C106" s="9" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="D106" s="9"/>
       <c r="E106" s="9"/>
@@ -7659,30 +8070,73 @@
     </row>
     <row r="107" spans="2:9" ht="32.25" thickBot="1">
       <c r="B107" s="8" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="C107" s="9" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="D107" s="9"/>
       <c r="E107" s="9"/>
       <c r="F107" s="9"/>
       <c r="G107" s="9"/>
       <c r="H107" s="9"/>
-      <c r="I107" s="11"/>
+      <c r="I107" s="9"/>
+    </row>
+    <row r="108" spans="2:9" ht="32.25" thickBot="1">
+      <c r="B108" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="C108" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="D108" s="9"/>
+      <c r="E108" s="9"/>
+      <c r="F108" s="9"/>
+      <c r="G108" s="9"/>
+      <c r="H108" s="9"/>
+      <c r="I108" s="9"/>
+    </row>
+    <row r="109" spans="2:9" ht="32.25" thickBot="1">
+      <c r="B109" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="C109" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="D109" s="9"/>
+      <c r="E109" s="9"/>
+      <c r="F109" s="9"/>
+      <c r="G109" s="9"/>
+      <c r="H109" s="9"/>
+      <c r="I109" s="9"/>
+    </row>
+    <row r="110" spans="2:9" ht="32.25" thickBot="1">
+      <c r="B110" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="C110" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="D110" s="9"/>
+      <c r="E110" s="9"/>
+      <c r="F110" s="9"/>
+      <c r="G110" s="9"/>
+      <c r="H110" s="9"/>
+      <c r="I110" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
     <mergeCell ref="G1:N3"/>
     <mergeCell ref="A7:R23"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="I29:I30"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="L27:Q28"/>
-    <mergeCell ref="B35:I35"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="I32:I33"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="L30:Q31"/>
+    <mergeCell ref="B38:I38"/>
+    <mergeCell ref="A24:R26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Latest DFMEA files of AMT project.
</commit_message>
<xml_diff>
--- a/AMT HALL EFFECT/05_Documents/FMEA/BOUNDARY_DIAGRAM_AMT.xlsx
+++ b/AMT HALL EFFECT/05_Documents/FMEA/BOUNDARY_DIAGRAM_AMT.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6255"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6255" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BD_AMT" sheetId="1" r:id="rId1"/>
@@ -1097,6 +1097,14 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1129,14 +1137,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4331,7 +4331,7 @@
         <xdr:cNvPr id="47" name="Text 52">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5458,6 +5458,63 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>6037</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>57493</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>672354</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>44825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="48" name="Rectangle 47"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5989978" y="4248493"/>
+          <a:ext cx="666317" cy="177832"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100"/>
+            <a:t>T(-2)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -5728,7 +5785,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
@@ -5741,128 +5798,128 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
       <c r="S1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="T1" s="24" t="s">
+      <c r="T1" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:20">
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
       <c r="S2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="T2" s="23">
+      <c r="T2" s="12">
         <v>43747</v>
       </c>
     </row>
     <row r="3" spans="1:20">
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
     </row>
     <row r="7" spans="1:20">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16"/>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="16"/>
-      <c r="R7" s="16"/>
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="18"/>
+      <c r="Q7" s="18"/>
+      <c r="R7" s="18"/>
     </row>
     <row r="8" spans="1:20">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="16"/>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="16"/>
-      <c r="R8" s="16"/>
+      <c r="A8" s="18"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="18"/>
+      <c r="Q8" s="18"/>
+      <c r="R8" s="18"/>
     </row>
     <row r="9" spans="1:20">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="16"/>
-      <c r="R9" s="16"/>
+      <c r="A9" s="18"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="18"/>
+      <c r="Q9" s="18"/>
+      <c r="R9" s="18"/>
     </row>
     <row r="10" spans="1:20">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="16"/>
-      <c r="N10" s="16"/>
-      <c r="O10" s="16"/>
-      <c r="P10" s="16"/>
-      <c r="Q10" s="16"/>
-      <c r="R10" s="16"/>
+      <c r="A10" s="18"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="18"/>
       <c r="S10" s="2" t="s">
         <v>1</v>
       </c>
@@ -5871,435 +5928,435 @@
       </c>
     </row>
     <row r="11" spans="1:20">
-      <c r="A11" s="16"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="16"/>
-      <c r="N11" s="16"/>
-      <c r="O11" s="16"/>
-      <c r="P11" s="16"/>
-      <c r="Q11" s="16"/>
-      <c r="R11" s="16"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="18"/>
+      <c r="Q11" s="18"/>
+      <c r="R11" s="18"/>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
     </row>
     <row r="12" spans="1:20">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="16"/>
-      <c r="N12" s="16"/>
-      <c r="O12" s="16"/>
-      <c r="P12" s="16"/>
-      <c r="Q12" s="16"/>
-      <c r="R12" s="16"/>
+      <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
+      <c r="P12" s="18"/>
+      <c r="Q12" s="18"/>
+      <c r="R12" s="18"/>
       <c r="S12" s="1"/>
       <c r="T12" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:20">
-      <c r="A13" s="16"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="16"/>
-      <c r="N13" s="16"/>
-      <c r="O13" s="16"/>
-      <c r="P13" s="16"/>
-      <c r="Q13" s="16"/>
-      <c r="R13" s="16"/>
+      <c r="A13" s="18"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="18"/>
+      <c r="O13" s="18"/>
+      <c r="P13" s="18"/>
+      <c r="Q13" s="18"/>
+      <c r="R13" s="18"/>
       <c r="S13" s="1"/>
       <c r="T13" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:20">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="16"/>
-      <c r="N14" s="16"/>
-      <c r="O14" s="16"/>
-      <c r="P14" s="16"/>
-      <c r="Q14" s="16"/>
-      <c r="R14" s="16"/>
-      <c r="S14" s="15"/>
-      <c r="T14" s="14" t="s">
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="18"/>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="18"/>
+      <c r="R14" s="18"/>
+      <c r="S14" s="17"/>
+      <c r="T14" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:20">
-      <c r="A15" s="16"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="16"/>
-      <c r="N15" s="16"/>
-      <c r="O15" s="16"/>
-      <c r="P15" s="16"/>
-      <c r="Q15" s="16"/>
-      <c r="R15" s="16"/>
-      <c r="S15" s="15"/>
-      <c r="T15" s="14"/>
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="18"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="18"/>
+      <c r="S15" s="17"/>
+      <c r="T15" s="16"/>
     </row>
     <row r="16" spans="1:20">
-      <c r="A16" s="16"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="16"/>
-      <c r="N16" s="16"/>
-      <c r="O16" s="16"/>
-      <c r="P16" s="16"/>
-      <c r="Q16" s="16"/>
-      <c r="R16" s="16"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="18"/>
+      <c r="O16" s="18"/>
+      <c r="P16" s="18"/>
+      <c r="Q16" s="18"/>
+      <c r="R16" s="18"/>
       <c r="S16" s="1"/>
       <c r="T16" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:20">
-      <c r="A17" s="16"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16"/>
-      <c r="L17" s="16"/>
-      <c r="M17" s="16"/>
-      <c r="N17" s="16"/>
-      <c r="O17" s="16"/>
-      <c r="P17" s="16"/>
-      <c r="Q17" s="16"/>
-      <c r="R17" s="16"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="18"/>
+      <c r="O17" s="18"/>
+      <c r="P17" s="18"/>
+      <c r="Q17" s="18"/>
+      <c r="R17" s="18"/>
       <c r="S17" s="1"/>
       <c r="T17" s="4" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="18" spans="1:20">
-      <c r="A18" s="16"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="16"/>
-      <c r="L18" s="16"/>
-      <c r="M18" s="16"/>
-      <c r="N18" s="16"/>
-      <c r="O18" s="16"/>
-      <c r="P18" s="16"/>
-      <c r="Q18" s="16"/>
-      <c r="R18" s="16"/>
+      <c r="A18" s="18"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="18"/>
+      <c r="N18" s="18"/>
+      <c r="O18" s="18"/>
+      <c r="P18" s="18"/>
+      <c r="Q18" s="18"/>
+      <c r="R18" s="18"/>
     </row>
     <row r="19" spans="1:20">
-      <c r="A19" s="16"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16"/>
-      <c r="L19" s="16"/>
-      <c r="M19" s="16"/>
-      <c r="N19" s="16"/>
-      <c r="O19" s="16"/>
-      <c r="P19" s="16"/>
-      <c r="Q19" s="16"/>
-      <c r="R19" s="16"/>
+      <c r="A19" s="18"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="18"/>
+      <c r="Q19" s="18"/>
+      <c r="R19" s="18"/>
     </row>
     <row r="20" spans="1:20">
-      <c r="A20" s="16"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="16"/>
-      <c r="L20" s="16"/>
-      <c r="M20" s="16"/>
-      <c r="N20" s="16"/>
-      <c r="O20" s="16"/>
-      <c r="P20" s="16"/>
-      <c r="Q20" s="16"/>
-      <c r="R20" s="16"/>
+      <c r="A20" s="18"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="18"/>
+      <c r="O20" s="18"/>
+      <c r="P20" s="18"/>
+      <c r="Q20" s="18"/>
+      <c r="R20" s="18"/>
     </row>
     <row r="21" spans="1:20">
-      <c r="A21" s="16"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
-      <c r="L21" s="16"/>
-      <c r="M21" s="16"/>
-      <c r="N21" s="16"/>
-      <c r="O21" s="16"/>
-      <c r="P21" s="16"/>
-      <c r="Q21" s="16"/>
-      <c r="R21" s="16"/>
+      <c r="A21" s="18"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="18"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="18"/>
+      <c r="Q21" s="18"/>
+      <c r="R21" s="18"/>
     </row>
     <row r="22" spans="1:20">
-      <c r="A22" s="16"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="16"/>
-      <c r="L22" s="16"/>
-      <c r="M22" s="16"/>
-      <c r="N22" s="16"/>
-      <c r="O22" s="16"/>
-      <c r="P22" s="16"/>
-      <c r="Q22" s="16"/>
-      <c r="R22" s="16"/>
+      <c r="A22" s="18"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="18"/>
+      <c r="P22" s="18"/>
+      <c r="Q22" s="18"/>
+      <c r="R22" s="18"/>
     </row>
     <row r="23" spans="1:20">
-      <c r="A23" s="16"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16"/>
-      <c r="L23" s="16"/>
-      <c r="M23" s="16"/>
-      <c r="N23" s="16"/>
-      <c r="O23" s="16"/>
-      <c r="P23" s="16"/>
-      <c r="Q23" s="16"/>
-      <c r="R23" s="16"/>
+      <c r="A23" s="18"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="18"/>
+      <c r="Q23" s="18"/>
+      <c r="R23" s="18"/>
     </row>
     <row r="24" spans="1:20">
-      <c r="A24" s="16"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="16"/>
-      <c r="L24" s="16"/>
-      <c r="M24" s="16"/>
-      <c r="N24" s="16"/>
-      <c r="O24" s="16"/>
-      <c r="P24" s="16"/>
-      <c r="Q24" s="16"/>
-      <c r="R24" s="16"/>
-      <c r="S24" s="16"/>
+      <c r="A24" s="18"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="18"/>
+      <c r="P24" s="18"/>
+      <c r="Q24" s="18"/>
+      <c r="R24" s="18"/>
+      <c r="S24" s="18"/>
     </row>
     <row r="25" spans="1:20">
-      <c r="A25" s="16"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="16"/>
-      <c r="K25" s="16"/>
-      <c r="L25" s="16"/>
-      <c r="M25" s="16"/>
-      <c r="N25" s="16"/>
-      <c r="O25" s="16"/>
-      <c r="P25" s="16"/>
-      <c r="Q25" s="16"/>
-      <c r="R25" s="16"/>
-      <c r="S25" s="16"/>
+      <c r="A25" s="18"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="18"/>
+      <c r="N25" s="18"/>
+      <c r="O25" s="18"/>
+      <c r="P25" s="18"/>
+      <c r="Q25" s="18"/>
+      <c r="R25" s="18"/>
+      <c r="S25" s="18"/>
     </row>
     <row r="26" spans="1:20">
-      <c r="A26" s="16"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="16"/>
-      <c r="L26" s="16"/>
-      <c r="M26" s="16"/>
-      <c r="N26" s="16"/>
-      <c r="O26" s="16"/>
-      <c r="P26" s="16"/>
-      <c r="Q26" s="16"/>
-      <c r="R26" s="16"/>
-      <c r="S26" s="16"/>
+      <c r="A26" s="18"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="18"/>
+      <c r="P26" s="18"/>
+      <c r="Q26" s="18"/>
+      <c r="R26" s="18"/>
+      <c r="S26" s="18"/>
     </row>
     <row r="27" spans="1:20">
-      <c r="A27" s="16"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="16"/>
-      <c r="J27" s="16"/>
-      <c r="K27" s="16"/>
-      <c r="L27" s="16"/>
-      <c r="M27" s="16"/>
-      <c r="N27" s="16"/>
-      <c r="O27" s="16"/>
-      <c r="P27" s="16"/>
-      <c r="Q27" s="16"/>
-      <c r="R27" s="16"/>
-      <c r="S27" s="16"/>
+      <c r="A27" s="18"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18"/>
+      <c r="M27" s="18"/>
+      <c r="N27" s="18"/>
+      <c r="O27" s="18"/>
+      <c r="P27" s="18"/>
+      <c r="Q27" s="18"/>
+      <c r="R27" s="18"/>
+      <c r="S27" s="18"/>
     </row>
     <row r="28" spans="1:20">
-      <c r="A28" s="16"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="16"/>
-      <c r="K28" s="16"/>
-      <c r="L28" s="16"/>
-      <c r="M28" s="16"/>
-      <c r="N28" s="16"/>
-      <c r="O28" s="16"/>
-      <c r="P28" s="16"/>
-      <c r="Q28" s="16"/>
-      <c r="R28" s="16"/>
-      <c r="S28" s="16"/>
+      <c r="A28" s="18"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18"/>
+      <c r="M28" s="18"/>
+      <c r="N28" s="18"/>
+      <c r="O28" s="18"/>
+      <c r="P28" s="18"/>
+      <c r="Q28" s="18"/>
+      <c r="R28" s="18"/>
+      <c r="S28" s="18"/>
     </row>
     <row r="29" spans="1:20">
-      <c r="A29" s="16"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="16"/>
-      <c r="L29" s="16"/>
-      <c r="M29" s="16"/>
-      <c r="N29" s="16"/>
-      <c r="O29" s="16"/>
-      <c r="P29" s="16"/>
-      <c r="Q29" s="16"/>
-      <c r="R29" s="16"/>
-      <c r="S29" s="16"/>
+      <c r="A29" s="18"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="18"/>
+      <c r="M29" s="18"/>
+      <c r="N29" s="18"/>
+      <c r="O29" s="18"/>
+      <c r="P29" s="18"/>
+      <c r="Q29" s="18"/>
+      <c r="R29" s="18"/>
+      <c r="S29" s="18"/>
     </row>
     <row r="30" spans="1:20">
-      <c r="A30" s="16"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="16"/>
-      <c r="K30" s="16"/>
-      <c r="L30" s="16"/>
-      <c r="M30" s="16"/>
-      <c r="N30" s="16"/>
-      <c r="O30" s="16"/>
-      <c r="P30" s="16"/>
-      <c r="Q30" s="16"/>
-      <c r="R30" s="16"/>
-      <c r="S30" s="16"/>
+      <c r="A30" s="18"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="18"/>
+      <c r="M30" s="18"/>
+      <c r="N30" s="18"/>
+      <c r="O30" s="18"/>
+      <c r="P30" s="18"/>
+      <c r="Q30" s="18"/>
+      <c r="R30" s="18"/>
+      <c r="S30" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -6319,8 +6376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T110"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T12" sqref="T12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6344,16 +6401,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
       <c r="S1" s="5" t="s">
         <v>7</v>
       </c>
@@ -6362,14 +6419,14 @@
       </c>
     </row>
     <row r="2" spans="1:20">
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
       <c r="S2" s="5" t="s">
         <v>9</v>
       </c>
@@ -6378,414 +6435,414 @@
       </c>
     </row>
     <row r="3" spans="1:20">
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
     </row>
     <row r="7" spans="1:20">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16"/>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="16"/>
-      <c r="R7" s="16"/>
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="18"/>
+      <c r="Q7" s="18"/>
+      <c r="R7" s="18"/>
     </row>
     <row r="8" spans="1:20">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="16"/>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="16"/>
-      <c r="R8" s="16"/>
+      <c r="A8" s="18"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="18"/>
+      <c r="Q8" s="18"/>
+      <c r="R8" s="18"/>
     </row>
     <row r="9" spans="1:20">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="16"/>
-      <c r="R9" s="16"/>
+      <c r="A9" s="18"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="18"/>
+      <c r="Q9" s="18"/>
+      <c r="R9" s="18"/>
     </row>
     <row r="10" spans="1:20">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="16"/>
-      <c r="N10" s="16"/>
-      <c r="O10" s="16"/>
-      <c r="P10" s="16"/>
-      <c r="Q10" s="16"/>
-      <c r="R10" s="16"/>
+      <c r="A10" s="18"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="18"/>
     </row>
     <row r="11" spans="1:20">
-      <c r="A11" s="16"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="16"/>
-      <c r="N11" s="16"/>
-      <c r="O11" s="16"/>
-      <c r="P11" s="16"/>
-      <c r="Q11" s="16"/>
-      <c r="R11" s="16"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="18"/>
+      <c r="Q11" s="18"/>
+      <c r="R11" s="18"/>
     </row>
     <row r="12" spans="1:20">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="16"/>
-      <c r="N12" s="16"/>
-      <c r="O12" s="16"/>
-      <c r="P12" s="16"/>
-      <c r="Q12" s="16"/>
-      <c r="R12" s="16"/>
+      <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
+      <c r="P12" s="18"/>
+      <c r="Q12" s="18"/>
+      <c r="R12" s="18"/>
     </row>
     <row r="13" spans="1:20">
-      <c r="A13" s="16"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="16"/>
-      <c r="N13" s="16"/>
-      <c r="O13" s="16"/>
-      <c r="P13" s="16"/>
-      <c r="Q13" s="16"/>
-      <c r="R13" s="16"/>
+      <c r="A13" s="18"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="18"/>
+      <c r="O13" s="18"/>
+      <c r="P13" s="18"/>
+      <c r="Q13" s="18"/>
+      <c r="R13" s="18"/>
     </row>
     <row r="14" spans="1:20">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="16"/>
-      <c r="N14" s="16"/>
-      <c r="O14" s="16"/>
-      <c r="P14" s="16"/>
-      <c r="Q14" s="16"/>
-      <c r="R14" s="16"/>
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="18"/>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="18"/>
+      <c r="R14" s="18"/>
     </row>
     <row r="15" spans="1:20">
-      <c r="A15" s="16"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="16"/>
-      <c r="N15" s="16"/>
-      <c r="O15" s="16"/>
-      <c r="P15" s="16"/>
-      <c r="Q15" s="16"/>
-      <c r="R15" s="16"/>
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="18"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="18"/>
     </row>
     <row r="16" spans="1:20">
-      <c r="A16" s="16"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="16"/>
-      <c r="N16" s="16"/>
-      <c r="O16" s="16"/>
-      <c r="P16" s="16"/>
-      <c r="Q16" s="16"/>
-      <c r="R16" s="16"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="18"/>
+      <c r="O16" s="18"/>
+      <c r="P16" s="18"/>
+      <c r="Q16" s="18"/>
+      <c r="R16" s="18"/>
     </row>
     <row r="17" spans="1:18">
-      <c r="A17" s="16"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16"/>
-      <c r="L17" s="16"/>
-      <c r="M17" s="16"/>
-      <c r="N17" s="16"/>
-      <c r="O17" s="16"/>
-      <c r="P17" s="16"/>
-      <c r="Q17" s="16"/>
-      <c r="R17" s="16"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="18"/>
+      <c r="O17" s="18"/>
+      <c r="P17" s="18"/>
+      <c r="Q17" s="18"/>
+      <c r="R17" s="18"/>
     </row>
     <row r="18" spans="1:18">
-      <c r="A18" s="16"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="16"/>
-      <c r="L18" s="16"/>
-      <c r="M18" s="16"/>
-      <c r="N18" s="16"/>
-      <c r="O18" s="16"/>
-      <c r="P18" s="16"/>
-      <c r="Q18" s="16"/>
-      <c r="R18" s="16"/>
+      <c r="A18" s="18"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="18"/>
+      <c r="N18" s="18"/>
+      <c r="O18" s="18"/>
+      <c r="P18" s="18"/>
+      <c r="Q18" s="18"/>
+      <c r="R18" s="18"/>
     </row>
     <row r="19" spans="1:18">
-      <c r="A19" s="16"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16"/>
-      <c r="L19" s="16"/>
-      <c r="M19" s="16"/>
-      <c r="N19" s="16"/>
-      <c r="O19" s="16"/>
-      <c r="P19" s="16"/>
-      <c r="Q19" s="16"/>
-      <c r="R19" s="16"/>
+      <c r="A19" s="18"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="18"/>
+      <c r="Q19" s="18"/>
+      <c r="R19" s="18"/>
     </row>
     <row r="20" spans="1:18">
-      <c r="A20" s="16"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="16"/>
-      <c r="L20" s="16"/>
-      <c r="M20" s="16"/>
-      <c r="N20" s="16"/>
-      <c r="O20" s="16"/>
-      <c r="P20" s="16"/>
-      <c r="Q20" s="16"/>
-      <c r="R20" s="16"/>
+      <c r="A20" s="18"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="18"/>
+      <c r="O20" s="18"/>
+      <c r="P20" s="18"/>
+      <c r="Q20" s="18"/>
+      <c r="R20" s="18"/>
     </row>
     <row r="21" spans="1:18">
-      <c r="A21" s="16"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
-      <c r="L21" s="16"/>
-      <c r="M21" s="16"/>
-      <c r="N21" s="16"/>
-      <c r="O21" s="16"/>
-      <c r="P21" s="16"/>
-      <c r="Q21" s="16"/>
-      <c r="R21" s="16"/>
+      <c r="A21" s="18"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="18"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="18"/>
+      <c r="Q21" s="18"/>
+      <c r="R21" s="18"/>
     </row>
     <row r="22" spans="1:18">
-      <c r="A22" s="16"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="16"/>
-      <c r="L22" s="16"/>
-      <c r="M22" s="16"/>
-      <c r="N22" s="16"/>
-      <c r="O22" s="16"/>
-      <c r="P22" s="16"/>
-      <c r="Q22" s="16"/>
-      <c r="R22" s="16"/>
+      <c r="A22" s="18"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="18"/>
+      <c r="P22" s="18"/>
+      <c r="Q22" s="18"/>
+      <c r="R22" s="18"/>
     </row>
     <row r="23" spans="1:18">
-      <c r="A23" s="16"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16"/>
-      <c r="L23" s="16"/>
-      <c r="M23" s="16"/>
-      <c r="N23" s="16"/>
-      <c r="O23" s="16"/>
-      <c r="P23" s="16"/>
-      <c r="Q23" s="16"/>
-      <c r="R23" s="16"/>
+      <c r="A23" s="18"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="18"/>
+      <c r="Q23" s="18"/>
+      <c r="R23" s="18"/>
     </row>
     <row r="24" spans="1:18">
-      <c r="A24" s="16"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="16"/>
-      <c r="L24" s="16"/>
-      <c r="M24" s="16"/>
-      <c r="N24" s="16"/>
-      <c r="O24" s="16"/>
-      <c r="P24" s="16"/>
-      <c r="Q24" s="16"/>
-      <c r="R24" s="16"/>
+      <c r="A24" s="18"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="18"/>
+      <c r="P24" s="18"/>
+      <c r="Q24" s="18"/>
+      <c r="R24" s="18"/>
     </row>
     <row r="25" spans="1:18">
-      <c r="A25" s="16"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="16"/>
-      <c r="K25" s="16"/>
-      <c r="L25" s="16"/>
-      <c r="M25" s="16"/>
-      <c r="N25" s="16"/>
-      <c r="O25" s="16"/>
-      <c r="P25" s="16"/>
-      <c r="Q25" s="16"/>
-      <c r="R25" s="16"/>
+      <c r="A25" s="18"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="18"/>
+      <c r="N25" s="18"/>
+      <c r="O25" s="18"/>
+      <c r="P25" s="18"/>
+      <c r="Q25" s="18"/>
+      <c r="R25" s="18"/>
     </row>
     <row r="26" spans="1:18">
-      <c r="A26" s="16"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="16"/>
-      <c r="L26" s="16"/>
-      <c r="M26" s="16"/>
-      <c r="N26" s="16"/>
-      <c r="O26" s="16"/>
-      <c r="P26" s="16"/>
-      <c r="Q26" s="16"/>
-      <c r="R26" s="16"/>
+      <c r="A26" s="18"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="18"/>
+      <c r="P26" s="18"/>
+      <c r="Q26" s="18"/>
+      <c r="R26" s="18"/>
     </row>
     <row r="28" spans="1:18">
       <c r="H28" s="2" t="s">
@@ -6804,36 +6861,36 @@
       <c r="I30" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="L30" s="21" t="s">
+      <c r="L30" s="23" t="s">
         <v>283</v>
       </c>
-      <c r="M30" s="21"/>
-      <c r="N30" s="21"/>
-      <c r="O30" s="21"/>
-      <c r="P30" s="21"/>
-      <c r="Q30" s="21"/>
+      <c r="M30" s="23"/>
+      <c r="N30" s="23"/>
+      <c r="O30" s="23"/>
+      <c r="P30" s="23"/>
+      <c r="Q30" s="23"/>
     </row>
     <row r="31" spans="1:18">
       <c r="H31" s="1"/>
       <c r="I31" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="L31" s="21"/>
-      <c r="M31" s="21"/>
-      <c r="N31" s="21"/>
-      <c r="O31" s="21"/>
-      <c r="P31" s="21"/>
-      <c r="Q31" s="21"/>
+      <c r="L31" s="23"/>
+      <c r="M31" s="23"/>
+      <c r="N31" s="23"/>
+      <c r="O31" s="23"/>
+      <c r="P31" s="23"/>
+      <c r="Q31" s="23"/>
     </row>
     <row r="32" spans="1:18">
-      <c r="H32" s="15"/>
-      <c r="I32" s="17" t="s">
+      <c r="H32" s="17"/>
+      <c r="I32" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="33" spans="2:9" ht="32.25" customHeight="1">
-      <c r="H33" s="15"/>
-      <c r="I33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="19"/>
     </row>
     <row r="34" spans="2:9">
       <c r="H34" s="1"/>
@@ -6849,34 +6906,34 @@
     </row>
     <row r="37" spans="2:9" ht="15.75" thickBot="1"/>
     <row r="38" spans="2:9" ht="16.5" thickBot="1">
-      <c r="B38" s="18" t="s">
+      <c r="B38" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C38" s="22"/>
-      <c r="D38" s="22"/>
-      <c r="E38" s="22"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="22"/>
-      <c r="I38" s="19"/>
+      <c r="C38" s="24"/>
+      <c r="D38" s="24"/>
+      <c r="E38" s="24"/>
+      <c r="F38" s="24"/>
+      <c r="G38" s="24"/>
+      <c r="H38" s="24"/>
+      <c r="I38" s="21"/>
     </row>
     <row r="39" spans="2:9" ht="16.5" thickBot="1">
-      <c r="B39" s="18" t="s">
+      <c r="B39" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C39" s="19"/>
-      <c r="D39" s="20" t="s">
+      <c r="C39" s="21"/>
+      <c r="D39" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="E39" s="19"/>
-      <c r="F39" s="20" t="s">
+      <c r="E39" s="21"/>
+      <c r="F39" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="G39" s="19"/>
-      <c r="H39" s="20" t="s">
+      <c r="G39" s="21"/>
+      <c r="H39" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="I39" s="19"/>
+      <c r="I39" s="21"/>
     </row>
     <row r="40" spans="2:9" ht="32.25" thickBot="1">
       <c r="B40" s="8" t="s">

</xml_diff>